<commit_message>
matriz de rastreamento finalizada
</commit_message>
<xml_diff>
--- a/Documentação/Documentos/backlog.xlsx
+++ b/Documentação/Documentos/backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbiza\OneDrive\Área de Trabalho\TEST\site-institucional\Documentação\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B0E5F0-C40F-45D0-A77D-2FDF5F7AB9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CFFD79-7FD8-4EA5-BBB7-9C1E1D591AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{20733E76-3990-4A04-89D2-BEA7BDE5C0C7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="114">
   <si>
     <t>Requisitos</t>
   </si>
@@ -212,15 +212,6 @@
     <t>LUX002 / UST001</t>
   </si>
   <si>
-    <t xml:space="preserve"> UST010</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LUX001</t>
-  </si>
-  <si>
-    <t>UST008</t>
-  </si>
-  <si>
     <t>UST006</t>
   </si>
   <si>
@@ -269,9 +260,6 @@
     <t>Tela que solicita e-mail e senha do usuário e dependendo da hierarquia cadastrada da acesso ao painel de gráficos (hierarquia baixa) e da acesso ao controle de cadastro de funcionários(visualizar,cadastrar, editar e excluir.)</t>
   </si>
   <si>
-    <t>Tela para que o usuário possa realizar o cadastro dos demais usuários que terão controle hierárquico menor no uso do aplicativo.(conectado a API NodeJS)</t>
-  </si>
-  <si>
     <t>Tela para que o usuário possa realizar o cadastro da empresa e do usuário ADM. (conectado a API NodeJS)</t>
   </si>
   <si>
@@ -287,15 +275,9 @@
     <t>revisado por aeris e brudney</t>
   </si>
   <si>
-    <t>Nesta tela, o usuário (hierarquia alta) poderá ter acesso as informações cadastradas de cada funcionário, além de poder visualizar,cadastrar, editar e excluir, se necessário.</t>
-  </si>
-  <si>
     <t>Página mostrando as principais dúvidas e suas resoluções, onde também é possível fazer solicitações de suporte ( conexão Helpdesk) à nossa empresa.</t>
   </si>
   <si>
-    <t>Conexão ao programa de suporte externo(helpdesk) conectado diretamente a tela de ajuda.</t>
-  </si>
-  <si>
     <t>Revisado por aeris</t>
   </si>
   <si>
@@ -305,9 +287,6 @@
     <t>O banco fornece os dados de hardware para serem enviados para a dashboard.(através de NodeJS)</t>
   </si>
   <si>
-    <t>A aplicação, será feita em Kotlin, Python e Java.</t>
-  </si>
-  <si>
     <t>Captura os dados de IP (pra confirmação), Rede(download e upload) em Mega com data e hora, e insere no banco da dados na tabela 'Dados capturados' .</t>
   </si>
   <si>
@@ -323,10 +302,82 @@
     <t>Cruzamento de informações</t>
   </si>
   <si>
-    <t>Processador e REDE - visualizar como o alto tráfego na REDE afeta na CPU.</t>
-  </si>
-  <si>
     <t>Importa o CSV da tabela 'RAW' do MySQL, excluindo valores nulos, transformando bytes em Mega e/ou Giga, realizar cruzamento de informações e gerar um gráfico baseado nisso.</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>sem referência</t>
+  </si>
+  <si>
+    <t>PPS002</t>
+  </si>
+  <si>
+    <t>UST009</t>
+  </si>
+  <si>
+    <t>UST008 / PPS001</t>
+  </si>
+  <si>
+    <t>UST003</t>
+  </si>
+  <si>
+    <t>UST004</t>
+  </si>
+  <si>
+    <t>UST001 / UST005</t>
+  </si>
+  <si>
+    <t>PPS003 / PPS002</t>
+  </si>
+  <si>
+    <t>Alertas</t>
+  </si>
+  <si>
+    <t>PPS003 / UST002 / UST007 / LUX001</t>
+  </si>
+  <si>
+    <t>Processador e REDE - visualizar como o alto tráfego na REDE afeta no desempenho da CPU.</t>
+  </si>
+  <si>
+    <t>UST003 / UST004</t>
+  </si>
+  <si>
+    <t>UST006 / LUX001 / UST001 / UST005</t>
+  </si>
+  <si>
+    <t>Conexão ao programa de suporte externo(helpdesk) conectado diretamente a tela de ajuda. O sistema utilizado será o Slack, por onde serão enviadas as notificações de alerta do distema e também onde será disponibilizada a comunicação entre os membos cadastrados no sistema da TEST.</t>
+  </si>
+  <si>
+    <t>A aplicação, será feita em Kotlin, Python e Java de forma a ser um executável.</t>
+  </si>
+  <si>
+    <t>Restrições e acessos</t>
+  </si>
+  <si>
+    <t>Hierarquia de cadastros realizada no banco MySQL onde os funcionários tem acesso de visualização e os usuários administradores em acesso de visualização e gerenciamento no cadastro dos funcionários.</t>
+  </si>
+  <si>
+    <t>Nesta tela, o usuário administrador (hierarquia alta) poderá ter acesso as informações cadastradas de cada funcionário, além de poder visualizar,cadastrar, editar e excluir, se necessário.</t>
+  </si>
+  <si>
+    <t>Tela para que o usuário possa realizar o cadastro dos demais usuários que terão controle hierárquico menor no uso do aplicativo de somente visualização.(conectado a API NodeJS)</t>
+  </si>
+  <si>
+    <t>Alertas externos no aplicativo slack(helpdesk) que notifiquem o componente que está fora das métricas estabelecidas de forma sucinta.</t>
+  </si>
+  <si>
+    <t>UST004 / UST001 / UST005</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LUX001 / UST010</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UST010 </t>
+  </si>
+  <si>
+    <t>PPS002 / UST009 / UST010 / LUX001</t>
   </si>
 </sst>
 </file>
@@ -444,7 +495,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -465,7 +516,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -812,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AAACF98-1C66-4789-BA04-529D16BEA6E3}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="71" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="71" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,8 +884,8 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:10" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>82</v>
+      <c r="A2" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>25</v>
@@ -866,16 +916,18 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="9">
+      <c r="A3" s="12"/>
+      <c r="B3" s="8">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>9</v>
@@ -894,16 +946,18 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="9">
+      <c r="A4" s="12"/>
+      <c r="B4" s="8">
         <v>2</v>
       </c>
-      <c r="C4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D4" s="4" t="s">
         <v>42</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>9</v>
@@ -922,16 +976,18 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="9">
+      <c r="A5" s="12"/>
+      <c r="B5" s="8">
         <v>3</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D5" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>9</v>
@@ -950,16 +1006,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="9">
+      <c r="A6" s="12"/>
+      <c r="B6" s="8">
         <v>4</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>91</v>
+      </c>
       <c r="D6" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>77</v>
+        <v>108</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>9</v>
@@ -978,16 +1036,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="9">
+      <c r="A7" s="12"/>
+      <c r="B7" s="8">
         <v>5</v>
       </c>
-      <c r="C7" s="7"/>
+      <c r="C7" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D7" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>9</v>
@@ -1005,17 +1065,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="9">
+    <row r="8" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="8">
         <v>6</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="11" t="s">
+        <v>102</v>
+      </c>
       <c r="D8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>80</v>
+      <c r="E8" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>9</v>
@@ -1033,17 +1095,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="9">
+    <row r="9" spans="1:10" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="8">
         <v>7</v>
       </c>
-      <c r="C9" s="7"/>
+      <c r="C9" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="D9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>79</v>
+        <v>66</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>75</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>9</v>
@@ -1062,16 +1126,18 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="9">
+      <c r="A10" s="12"/>
+      <c r="B10" s="8">
         <v>8</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D10" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>81</v>
+        <v>67</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>77</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>9</v>
@@ -1089,17 +1155,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="9">
-        <v>9</v>
-      </c>
-      <c r="C11" s="7"/>
+    <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="8">
+        <v>9</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>92</v>
+      </c>
       <c r="D11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>83</v>
+        <v>107</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>9</v>
@@ -1118,11 +1186,13 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="9">
+      <c r="A12" s="12"/>
+      <c r="B12" s="8">
         <v>10</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1146,16 +1216,18 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="9">
+      <c r="A13" s="12"/>
+      <c r="B13" s="8">
         <v>11</v>
       </c>
-      <c r="C13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="15" t="s">
-        <v>84</v>
+      <c r="E13" s="14" t="s">
+        <v>79</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>9</v>
@@ -1174,11 +1246,13 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
-      <c r="B14" s="9">
+      <c r="A14" s="12"/>
+      <c r="B14" s="8">
         <v>12</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D14" s="4" t="s">
         <v>18</v>
       </c>
@@ -1202,11 +1276,13 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
-      <c r="B15" s="9">
+      <c r="A15" s="12"/>
+      <c r="B15" s="8">
         <v>13</v>
       </c>
-      <c r="C15" s="7"/>
+      <c r="C15" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D15" s="4" t="s">
         <v>19</v>
       </c>
@@ -1229,17 +1305,19 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="9">
+    <row r="16" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="8">
         <v>14</v>
       </c>
-      <c r="C16" s="7"/>
+      <c r="C16" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="D16" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>85</v>
+        <v>103</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>9</v>
@@ -1257,17 +1335,19 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
-      <c r="B17" s="9">
+    <row r="17" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="8">
         <v>15</v>
       </c>
-      <c r="C17" s="7"/>
+      <c r="C17" s="11" t="s">
+        <v>99</v>
+      </c>
       <c r="D17" s="4" t="s">
-        <v>39</v>
+        <v>98</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>9</v>
@@ -1276,25 +1356,46 @@
         <v>32</v>
       </c>
       <c r="H17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="6">
+        <v>8</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="8">
+        <v>16</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I18" s="6">
         <v>3</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J18" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1303,107 +1404,90 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="I21" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="9">
-        <v>16</v>
-      </c>
-      <c r="C21" s="7" t="s">
+    <row r="22" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="8">
+        <v>17</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" s="6" t="s">
+      <c r="E22" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I22" s="6">
         <v>13</v>
       </c>
-      <c r="J21" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="13"/>
-      <c r="B22" s="9">
-        <v>17</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="6">
-        <v>8</v>
-      </c>
       <c r="J22" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="9">
+    <row r="23" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="8">
         <v>18</v>
       </c>
-      <c r="C23" s="7"/>
+      <c r="C23" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D23" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>88</v>
+        <v>61</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>81</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>9</v>
@@ -1422,54 +1506,54 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
-      <c r="B24" s="9">
+      <c r="A24" s="12"/>
+      <c r="B24" s="8">
         <v>19</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="6">
+        <v>8</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="8">
+        <v>20</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G24" s="6" t="s">
+      <c r="F25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I24" s="6">
-        <v>13</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
-      <c r="B25" s="9">
-        <v>20</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>45</v>
@@ -1481,17 +1565,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="9">
+    <row r="26" spans="1:10" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="8">
         <v>21</v>
       </c>
-      <c r="C26" s="12"/>
+      <c r="C26" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="D26" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>90</v>
+        <v>33</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>9</v>
@@ -1500,26 +1586,28 @@
         <v>32</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="I26" s="6">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="J26" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="9">
+    <row r="27" spans="1:10" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="8">
         <v>22</v>
       </c>
-      <c r="C27" s="12"/>
+      <c r="C27" s="11" t="s">
+        <v>95</v>
+      </c>
       <c r="D27" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>91</v>
+        <v>64</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>9</v>
@@ -1537,25 +1625,25 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
-      <c r="B28" s="9">
+    <row r="28" spans="1:10" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="12"/>
+      <c r="B28" s="8">
         <v>23</v>
       </c>
-      <c r="C28" s="12" t="s">
-        <v>58</v>
+      <c r="C28" s="11" t="s">
+        <v>96</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>40</v>
@@ -1567,17 +1655,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
-      <c r="B29" s="9">
+    <row r="29" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="B29" s="8">
         <v>24</v>
       </c>
-      <c r="C29" s="8"/>
+      <c r="C29" s="11" t="s">
+        <v>112</v>
+      </c>
       <c r="D29" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>9</v>
@@ -1595,17 +1685,19 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
-      <c r="B30" s="9">
+    <row r="30" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12"/>
+      <c r="B30" s="8">
         <v>25</v>
       </c>
-      <c r="C30" s="8"/>
+      <c r="C30" s="7" t="s">
+        <v>56</v>
+      </c>
       <c r="D30" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>9</v>
@@ -1614,28 +1706,28 @@
         <v>44</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I30" s="6">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J30" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="13"/>
-      <c r="B31" s="9">
+    <row r="31" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="8">
         <v>26</v>
       </c>
-      <c r="C31" s="12" t="s">
-        <v>59</v>
+      <c r="C31" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>9</v>
@@ -1644,142 +1736,148 @@
         <v>44</v>
       </c>
       <c r="H31" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="I31" s="6">
+        <v>5</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="12"/>
+      <c r="B32" s="8">
+        <v>27</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I31" s="6">
+      <c r="I32" s="6">
         <v>13</v>
       </c>
-      <c r="J31" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
-      <c r="B32" s="9">
-        <v>27</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D32" s="4" t="s">
+      <c r="J32" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="12"/>
+      <c r="B33" s="8">
+        <v>28</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D33" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G32" s="6" t="s">
+      <c r="F33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H33" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="6">
+      <c r="I33" s="6">
         <v>5</v>
       </c>
-      <c r="J32" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
-      <c r="B33" s="9">
-        <v>28</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="J33" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="12"/>
+      <c r="B34" s="8">
+        <v>29</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F34" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I33" s="6">
-        <v>8</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="9">
-        <v>29</v>
-      </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="E34" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>9</v>
       </c>
       <c r="G34" s="6" t="s">
         <v>44</v>
       </c>
       <c r="H34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I34" s="6">
+        <v>8</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="12"/>
+      <c r="B35" s="8">
+        <v>30</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E35" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H35" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I35" s="6">
         <v>13</v>
       </c>
-      <c r="J34" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="13"/>
-      <c r="B35" s="9">
-        <v>30</v>
-      </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I35" s="6">
-        <v>8</v>
-      </c>
       <c r="J35" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="9">
+    <row r="36" spans="1:10" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="12"/>
+      <c r="B36" s="8">
         <v>31</v>
       </c>
-      <c r="C36" s="8"/>
+      <c r="C36" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="D36" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>95</v>
+        <v>86</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>9</v>
@@ -1797,28 +1895,96 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B39" s="10" t="s">
+    <row r="37" spans="1:10" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="8">
+        <v>32</v>
+      </c>
+      <c r="C37" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E37" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I37" s="6">
+        <v>8</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="12"/>
+      <c r="B38" s="8">
+        <v>33</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I38" s="6">
+        <v>8</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C41" s="10" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B40" s="10" t="s">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C42" s="10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B41" s="10" t="s">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C43" s="10" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1828,6 +1994,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="58bd19be-68b1-440c-82af-6d4de24fec6c" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003236BA383373F9498A6F9C22979A1745" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0bf3bdad6f269cdb0c97dea15d0c6482">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="58bd19be-68b1-440c-82af-6d4de24fec6c" xmlns:ns4="3ffc9a63-5890-437d-bab6-67d84705b086" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="99d51bb674e47819d402eb0a523b7d3f" ns3:_="" ns4:_="">
     <xsd:import namespace="58bd19be-68b1-440c-82af-6d4de24fec6c"/>
@@ -2042,14 +2216,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="58bd19be-68b1-440c-82af-6d4de24fec6c" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2060,6 +2226,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCF05926-E130-461A-A1C5-9C974146D11D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3ffc9a63-5890-437d-bab6-67d84705b086"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="58bd19be-68b1-440c-82af-6d4de24fec6c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71C33E66-45E6-4074-8D53-095A0939F250}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2078,23 +2261,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCF05926-E130-461A-A1C5-9C974146D11D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3ffc9a63-5890-437d-bab6-67d84705b086"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="58bd19be-68b1-440c-82af-6d4de24fec6c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD4BB65A-7ADA-4649-93F2-A6878AA75E80}">
   <ds:schemaRefs>

</xml_diff>